<commit_message>
Initial skill extraction from jobs
</commit_message>
<xml_diff>
--- a/skills/Digital Skills.xlsx
+++ b/skills/Digital Skills.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/binxuan/Desktop/Projects/Skills Ontology/skills/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kongbinxuan/Desktop/skills-onthology-project/skills/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D84848-803F-0842-A18A-18291B95D482}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE92625-3DA1-D64F-9959-DC29D491D5C0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10800" yWindow="460" windowWidth="18000" windowHeight="16140" activeTab="2" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
+    <workbookView xWindow="10800" yWindow="460" windowWidth="18000" windowHeight="16140" activeTab="1" xr2:uid="{273D56F0-60F4-7D4D-B74A-F5CA8C152A80}"/>
   </bookViews>
   <sheets>
     <sheet name="Base" sheetId="1" r:id="rId1"/>
@@ -3095,7 +3095,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3106,7 +3106,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -3288,8 +3287,8 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{27EF683E-E617-FC45-A9F4-3737C17AF3B3}" name="Table13456" displayName="Table13456" ref="A1:B122" totalsRowShown="0">
   <autoFilter ref="A1:B122" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B17">
-    <sortCondition ref="B1:B17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B122">
+    <sortCondition ref="A1:A122"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4D657AA0-93DD-2941-AE44-71A11F855079}" name="Skill"/>
@@ -3302,8 +3301,8 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{387527DB-FE19-FC4D-ABB5-906E37E52660}" name="Table134567" displayName="Table134567" ref="A1:B287" totalsRowShown="0">
   <autoFilter ref="A1:B287" xr:uid="{70E2AE85-8354-604E-A8F5-BA1E0909D1D5}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B163">
-    <sortCondition ref="B1:B163"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B287">
+    <sortCondition ref="A1:A287"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{83C7801B-251E-164F-8C5A-E2D83147F54D}" name="Skill"/>
@@ -4192,8 +4191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC568B44-548B-D74F-B49B-DF829991C980}">
   <dimension ref="A1:B170"/>
   <sheetViews>
-    <sheetView topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="A171" sqref="A171"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5573,7 +5572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC367FE4-F21A-4B4E-A4D6-C29EEEBA6A4D}">
   <dimension ref="A1:B292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A241" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="B265" sqref="B265"/>
     </sheetView>
   </sheetViews>
@@ -7066,7 +7065,7 @@
       <c r="A186" s="2" t="s">
         <v>519</v>
       </c>
-      <c r="B186" s="11" t="s">
+      <c r="B186" s="10" t="s">
         <v>515</v>
       </c>
     </row>
@@ -7074,7 +7073,7 @@
       <c r="A187" s="2" t="s">
         <v>521</v>
       </c>
-      <c r="B187" s="11" t="s">
+      <c r="B187" s="10" t="s">
         <v>515</v>
       </c>
     </row>
@@ -7082,7 +7081,7 @@
       <c r="A188" s="2" t="s">
         <v>520</v>
       </c>
-      <c r="B188" s="11" t="s">
+      <c r="B188" s="10" t="s">
         <v>515</v>
       </c>
     </row>
@@ -9627,7 +9626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AB18F8-3BFD-6745-86FB-84FE740E519C}">
   <dimension ref="A1:B122"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
@@ -9646,407 +9645,407 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>177</v>
+        <v>671</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>618</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>662</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>637</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>227</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>986</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>613</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>612</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>672</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>618</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>986</v>
+        <v>669</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>637</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>264</v>
+        <v>842</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>840</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>179</v>
+        <v>673</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>618</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>180</v>
+        <v>625</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>637</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>183</v>
+        <v>622</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>621</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>185</v>
+        <v>637</v>
       </c>
       <c r="B12" t="s">
-        <v>178</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>265</v>
+        <v>626</v>
       </c>
       <c r="B13" t="s">
-        <v>264</v>
+        <v>637</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>266</v>
+        <v>627</v>
       </c>
       <c r="B14" t="s">
-        <v>264</v>
+        <v>637</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>187</v>
+        <v>621</v>
       </c>
       <c r="B15" t="s">
-        <v>186</v>
+        <v>618</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>186</v>
+        <v>674</v>
       </c>
       <c r="B16" t="s">
-        <v>179</v>
+        <v>618</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>227</v>
+        <v>628</v>
       </c>
       <c r="B17" t="s">
-        <v>986</v>
+        <v>637</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>597</v>
+        <v>182</v>
       </c>
       <c r="B18" t="s">
-        <v>596</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>598</v>
+        <v>181</v>
       </c>
       <c r="B19" t="s">
-        <v>597</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>599</v>
+        <v>178</v>
       </c>
       <c r="B20" t="s">
-        <v>597</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>600</v>
+        <v>986</v>
       </c>
       <c r="B21" t="s">
-        <v>597</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>601</v>
+        <v>264</v>
       </c>
       <c r="B22" t="s">
-        <v>597</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>602</v>
+        <v>266</v>
       </c>
       <c r="B23" t="s">
-        <v>597</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>605</v>
+        <v>265</v>
       </c>
       <c r="B24" t="s">
-        <v>602</v>
+        <v>264</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>604</v>
+        <v>675</v>
       </c>
       <c r="B25" t="s">
-        <v>602</v>
+        <v>618</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>603</v>
+        <v>668</v>
       </c>
       <c r="B26" t="s">
-        <v>602</v>
+        <v>637</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>606</v>
+        <v>667</v>
       </c>
       <c r="B27" t="s">
-        <v>596</v>
+        <v>637</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>607</v>
+        <v>657</v>
       </c>
       <c r="B28" t="s">
-        <v>606</v>
+        <v>638</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>610</v>
+        <v>639</v>
       </c>
       <c r="B29" t="s">
-        <v>606</v>
+        <v>638</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>608</v>
+        <v>692</v>
       </c>
       <c r="B30" t="s">
-        <v>606</v>
+        <v>689</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>609</v>
+        <v>617</v>
       </c>
       <c r="B31" t="s">
-        <v>606</v>
+        <v>615</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>611</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
-        <v>606</v>
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>612</v>
+        <v>187</v>
       </c>
       <c r="B33" t="s">
-        <v>596</v>
+        <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>613</v>
+        <v>605</v>
       </c>
       <c r="B34" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>614</v>
+        <v>604</v>
       </c>
       <c r="B35" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>615</v>
+        <v>656</v>
       </c>
       <c r="B36" t="s">
-        <v>612</v>
+        <v>647</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="B37" t="s">
-        <v>615</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>617</v>
+        <v>648</v>
       </c>
       <c r="B38" t="s">
-        <v>615</v>
+        <v>647</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>495</v>
+        <v>603</v>
       </c>
       <c r="B39" t="s">
-        <v>615</v>
+        <v>602</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>619</v>
+        <v>609</v>
       </c>
       <c r="B40" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>620</v>
+        <v>676</v>
       </c>
       <c r="B41" t="s">
-        <v>596</v>
+        <v>618</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>618</v>
+        <v>185</v>
       </c>
       <c r="B42" t="s">
-        <v>619</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>621</v>
+        <v>495</v>
       </c>
       <c r="B43" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="B44" t="s">
-        <v>621</v>
+        <v>637</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
       <c r="B45" t="s">
-        <v>621</v>
+        <v>637</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="B46" t="s">
-        <v>621</v>
+        <v>606</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>669</v>
+        <v>623</v>
       </c>
       <c r="B47" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>625</v>
+        <v>638</v>
       </c>
       <c r="B48" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>626</v>
+        <v>608</v>
       </c>
       <c r="B49" t="s">
-        <v>637</v>
+        <v>606</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>627</v>
+        <v>649</v>
       </c>
       <c r="B50" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>670</v>
+        <v>640</v>
       </c>
       <c r="B51" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>628</v>
+        <v>670</v>
       </c>
       <c r="B52" t="s">
         <v>637</v>
@@ -10054,143 +10053,143 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>668</v>
+        <v>179</v>
       </c>
       <c r="B53" t="s">
-        <v>637</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>667</v>
+        <v>841</v>
       </c>
       <c r="B54" t="s">
-        <v>637</v>
+        <v>840</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>666</v>
+        <v>616</v>
       </c>
       <c r="B55" t="s">
-        <v>637</v>
+        <v>615</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="B56" t="s">
-        <v>637</v>
+        <v>612</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>630</v>
+        <v>183</v>
       </c>
       <c r="B57" t="s">
-        <v>637</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>631</v>
+        <v>650</v>
       </c>
       <c r="B58" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>632</v>
+        <v>987</v>
       </c>
       <c r="B59" t="s">
-        <v>637</v>
+        <v>12</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>665</v>
+        <v>620</v>
       </c>
       <c r="B60" t="s">
-        <v>637</v>
+        <v>596</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>664</v>
+        <v>677</v>
       </c>
       <c r="B61" t="s">
-        <v>637</v>
+        <v>618</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>633</v>
+        <v>599</v>
       </c>
       <c r="B62" t="s">
-        <v>637</v>
+        <v>597</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
       <c r="B63" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>662</v>
+        <v>651</v>
       </c>
       <c r="B64" t="s">
-        <v>637</v>
+        <v>647</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>634</v>
+        <v>840</v>
       </c>
       <c r="B65" t="s">
-        <v>637</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>635</v>
+        <v>678</v>
       </c>
       <c r="B66" t="s">
-        <v>637</v>
+        <v>618</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>661</v>
+        <v>606</v>
       </c>
       <c r="B67" t="s">
-        <v>637</v>
+        <v>596</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>171</v>
+        <v>679</v>
       </c>
       <c r="B68" t="s">
-        <v>637</v>
+        <v>618</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>660</v>
+        <v>680</v>
       </c>
       <c r="B69" t="s">
-        <v>637</v>
+        <v>618</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>636</v>
+        <v>631</v>
       </c>
       <c r="B70" t="s">
         <v>637</v>
@@ -10198,7 +10197,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>659</v>
+        <v>666</v>
       </c>
       <c r="B71" t="s">
         <v>637</v>
@@ -10206,159 +10205,159 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>658</v>
+        <v>601</v>
       </c>
       <c r="B72" t="s">
-        <v>637</v>
+        <v>597</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>637</v>
+        <v>652</v>
       </c>
       <c r="B73" t="s">
-        <v>622</v>
+        <v>647</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
+        <v>655</v>
+      </c>
+      <c r="B74" t="s">
         <v>638</v>
-      </c>
-      <c r="B74" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>655</v>
+        <v>659</v>
       </c>
       <c r="B75" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>639</v>
+        <v>681</v>
       </c>
       <c r="B76" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>640</v>
+        <v>682</v>
       </c>
       <c r="B77" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>657</v>
+        <v>607</v>
       </c>
       <c r="B78" t="s">
-        <v>638</v>
+        <v>606</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>641</v>
+        <v>611</v>
       </c>
       <c r="B79" t="s">
-        <v>638</v>
+        <v>606</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>642</v>
+        <v>689</v>
       </c>
       <c r="B80" t="s">
-        <v>638</v>
+        <v>596</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>643</v>
+        <v>184</v>
       </c>
       <c r="B81" t="s">
-        <v>638</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>644</v>
+        <v>632</v>
       </c>
       <c r="B82" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>645</v>
+        <v>665</v>
       </c>
       <c r="B83" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>646</v>
+        <v>683</v>
       </c>
       <c r="B84" t="s">
-        <v>638</v>
+        <v>618</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="B85" t="s">
-        <v>624</v>
+        <v>638</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>656</v>
+        <v>990</v>
       </c>
       <c r="B86" t="s">
-        <v>647</v>
+        <v>12</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>648</v>
+        <v>612</v>
       </c>
       <c r="B87" t="s">
-        <v>647</v>
+        <v>596</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>649</v>
+        <v>664</v>
       </c>
       <c r="B88" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>650</v>
+        <v>684</v>
       </c>
       <c r="B89" t="s">
-        <v>647</v>
+        <v>618</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>651</v>
+        <v>685</v>
       </c>
       <c r="B90" t="s">
-        <v>647</v>
+        <v>618</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B91" t="s">
         <v>647</v>
@@ -10366,47 +10365,47 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>653</v>
+        <v>633</v>
       </c>
       <c r="B92" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>654</v>
+        <v>663</v>
       </c>
       <c r="B93" t="s">
-        <v>647</v>
+        <v>637</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>671</v>
+        <v>643</v>
       </c>
       <c r="B94" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>672</v>
+        <v>614</v>
       </c>
       <c r="B95" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>673</v>
+        <v>634</v>
       </c>
       <c r="B96" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>674</v>
+        <v>686</v>
       </c>
       <c r="B97" t="s">
         <v>618</v>
@@ -10414,87 +10413,87 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>675</v>
+        <v>177</v>
       </c>
       <c r="B98" t="s">
-        <v>618</v>
+        <v>12</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>676</v>
+        <v>635</v>
       </c>
       <c r="B99" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
       <c r="B100" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>678</v>
+        <v>690</v>
       </c>
       <c r="B101" t="s">
-        <v>618</v>
+        <v>689</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>679</v>
+        <v>654</v>
       </c>
       <c r="B102" t="s">
-        <v>618</v>
+        <v>647</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>680</v>
+        <v>644</v>
       </c>
       <c r="B103" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>681</v>
+        <v>645</v>
       </c>
       <c r="B104" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>682</v>
+        <v>171</v>
       </c>
       <c r="B105" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>683</v>
+        <v>660</v>
       </c>
       <c r="B106" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>684</v>
+        <v>636</v>
       </c>
       <c r="B107" t="s">
-        <v>618</v>
+        <v>637</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="B108" t="s">
         <v>618</v>
@@ -10502,18 +10501,18 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>686</v>
+        <v>646</v>
       </c>
       <c r="B109" t="s">
-        <v>618</v>
+        <v>638</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B110" t="s">
-        <v>618</v>
+        <v>287</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
@@ -10521,7 +10520,7 @@
         <v>688</v>
       </c>
       <c r="B111" t="s">
-        <v>287</v>
+        <v>618</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -10529,20 +10528,20 @@
         <v>688</v>
       </c>
       <c r="B112" t="s">
-        <v>618</v>
+        <v>597</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>688</v>
+        <v>618</v>
       </c>
       <c r="B113" t="s">
-        <v>597</v>
+        <v>619</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>689</v>
+        <v>597</v>
       </c>
       <c r="B114" t="s">
         <v>596</v>
@@ -10550,66 +10549,66 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>691</v>
+        <v>598</v>
       </c>
       <c r="B115" t="s">
-        <v>689</v>
+        <v>597</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>692</v>
+        <v>624</v>
       </c>
       <c r="B116" t="s">
-        <v>689</v>
+        <v>621</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>690</v>
+        <v>647</v>
       </c>
       <c r="B117" t="s">
-        <v>689</v>
+        <v>624</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>840</v>
+        <v>619</v>
       </c>
       <c r="B118" t="s">
-        <v>12</v>
+        <v>596</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>841</v>
+        <v>180</v>
       </c>
       <c r="B119" t="s">
-        <v>840</v>
+        <v>178</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>842</v>
+        <v>691</v>
       </c>
       <c r="B120" t="s">
-        <v>840</v>
+        <v>689</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>987</v>
+        <v>658</v>
       </c>
       <c r="B121" t="s">
-        <v>12</v>
+        <v>637</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>990</v>
+        <v>600</v>
       </c>
       <c r="B122" t="s">
-        <v>12</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -10624,7 +10623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82DCE302-5DE7-CD43-B663-062D99EF0251}">
   <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
@@ -10643,15 +10642,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
       <c r="B2" t="s">
-        <v>783</v>
+        <v>694</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>785</v>
+        <v>789</v>
       </c>
       <c r="B3" t="s">
         <v>783</v>
@@ -10659,7 +10658,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>791</v>
+        <v>785</v>
       </c>
       <c r="B4" t="s">
         <v>783</v>
@@ -10667,255 +10666,255 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>790</v>
-      </c>
-      <c r="B5" s="9" t="s">
+        <v>791</v>
+      </c>
+      <c r="B5" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>793</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>783</v>
+        <v>497</v>
+      </c>
+      <c r="B6" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>784</v>
+        <v>726</v>
       </c>
       <c r="B7" t="s">
-        <v>783</v>
+        <v>724</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>788</v>
+        <v>744</v>
       </c>
       <c r="B8" t="s">
-        <v>789</v>
+        <v>743</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>792</v>
+        <v>916</v>
       </c>
       <c r="B9" t="s">
-        <v>791</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>786</v>
+        <v>287</v>
       </c>
       <c r="B10" t="s">
-        <v>791</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>787</v>
+        <v>743</v>
       </c>
       <c r="B11" t="s">
-        <v>791</v>
+        <v>595</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>295</v>
+        <v>743</v>
       </c>
       <c r="B12" t="s">
-        <v>287</v>
+        <v>694</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>297</v>
+        <v>749</v>
       </c>
       <c r="B13" t="s">
-        <v>287</v>
+        <v>595</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>296</v>
+        <v>806</v>
       </c>
       <c r="B14" t="s">
-        <v>287</v>
+        <v>749</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>290</v>
+        <v>807</v>
       </c>
       <c r="B15" t="s">
-        <v>287</v>
+        <v>749</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>293</v>
+        <v>807</v>
       </c>
       <c r="B16" t="s">
-        <v>287</v>
+        <v>612</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>294</v>
+        <v>808</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>749</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>291</v>
+        <v>928</v>
       </c>
       <c r="B18" t="s">
-        <v>287</v>
+        <v>919</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>292</v>
+        <v>696</v>
       </c>
       <c r="B19" t="s">
-        <v>287</v>
+        <v>694</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>744</v>
+        <v>705</v>
       </c>
       <c r="B20" t="s">
-        <v>743</v>
+        <v>724</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>754</v>
+        <v>705</v>
       </c>
       <c r="B21" t="s">
-        <v>743</v>
+        <v>704</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>746</v>
+        <v>805</v>
       </c>
       <c r="B22" t="s">
-        <v>743</v>
+        <v>749</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>747</v>
+        <v>872</v>
       </c>
       <c r="B23" t="s">
-        <v>743</v>
+        <v>863</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>745</v>
+        <v>721</v>
       </c>
       <c r="B24" t="s">
-        <v>743</v>
+        <v>717</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>748</v>
+        <v>498</v>
       </c>
       <c r="B25" t="s">
-        <v>743</v>
+        <v>495</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>750</v>
+        <v>761</v>
       </c>
       <c r="B26" t="s">
-        <v>749</v>
+        <v>811</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>806</v>
+        <v>494</v>
       </c>
       <c r="B27" t="s">
-        <v>749</v>
+        <v>493</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>801</v>
+        <v>874</v>
       </c>
       <c r="B28" t="s">
-        <v>749</v>
+        <v>612</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>802</v>
+        <v>811</v>
       </c>
       <c r="B29" t="s">
-        <v>749</v>
+        <v>493</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>803</v>
+        <v>813</v>
       </c>
       <c r="B30" t="s">
-        <v>749</v>
+        <v>811</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>807</v>
-      </c>
-      <c r="B31" t="s">
-        <v>749</v>
+        <v>882</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>804</v>
+        <v>295</v>
       </c>
       <c r="B32" t="s">
-        <v>749</v>
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>805</v>
+        <v>709</v>
       </c>
       <c r="B33" t="s">
-        <v>749</v>
+        <v>704</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>808</v>
+        <v>710</v>
       </c>
       <c r="B34" t="s">
-        <v>749</v>
+        <v>704</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>810</v>
+        <v>711</v>
       </c>
       <c r="B35" t="s">
-        <v>811</v>
+        <v>704</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B36" t="s">
         <v>595</v>
@@ -10923,63 +10922,63 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>749</v>
+        <v>725</v>
       </c>
       <c r="B37" t="s">
-        <v>595</v>
+        <v>724</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>742</v>
+        <v>699</v>
       </c>
       <c r="B38" t="s">
-        <v>595</v>
+        <v>694</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>751</v>
+        <v>769</v>
       </c>
       <c r="B39" t="s">
-        <v>595</v>
+        <v>770</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>752</v>
+        <v>727</v>
       </c>
       <c r="B40" t="s">
-        <v>595</v>
+        <v>724</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>704</v>
-      </c>
-      <c r="B41" t="s">
-        <v>595</v>
+        <v>738</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="3" t="s">
-        <v>768</v>
+      <c r="A42" t="s">
+        <v>831</v>
       </c>
       <c r="B42" t="s">
-        <v>769</v>
+        <v>832</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>287</v>
+        <v>814</v>
       </c>
       <c r="B43" t="s">
-        <v>288</v>
+        <v>612</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>761</v>
+        <v>814</v>
       </c>
       <c r="B44" t="s">
         <v>811</v>
@@ -10987,23 +10986,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>763</v>
+        <v>814</v>
       </c>
       <c r="B45" t="s">
-        <v>493</v>
+        <v>749</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>767</v>
+        <v>867</v>
       </c>
       <c r="B46" t="s">
-        <v>493</v>
+        <v>863</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>766</v>
+        <v>763</v>
       </c>
       <c r="B47" t="s">
         <v>493</v>
@@ -11011,7 +11010,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>495</v>
+        <v>767</v>
       </c>
       <c r="B48" t="s">
         <v>493</v>
@@ -11019,15 +11018,15 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
       <c r="B49" t="s">
-        <v>493</v>
+        <v>768</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>493</v>
@@ -11035,130 +11034,130 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="B51" t="s">
-        <v>493</v>
+        <v>768</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>762</v>
+        <v>493</v>
       </c>
       <c r="B52" t="s">
-        <v>811</v>
+        <v>694</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>509</v>
+        <v>697</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>493</v>
+        <v>694</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>510</v>
+        <v>697</v>
       </c>
       <c r="B54" t="s">
-        <v>493</v>
+        <v>724</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>511</v>
+        <v>698</v>
       </c>
       <c r="B55" t="s">
-        <v>493</v>
+        <v>694</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>512</v>
+        <v>700</v>
       </c>
       <c r="B56" t="s">
-        <v>493</v>
+        <v>694</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="B57" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>811</v>
+        <v>898</v>
       </c>
       <c r="B58" t="s">
-        <v>493</v>
+        <v>906</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>735</v>
+        <v>833</v>
       </c>
       <c r="B59" t="s">
-        <v>740</v>
+        <v>832</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>500</v>
+        <v>835</v>
       </c>
       <c r="B60" t="s">
-        <v>30</v>
+        <v>834</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>706</v>
+        <v>795</v>
       </c>
       <c r="B61" t="s">
-        <v>707</v>
+        <v>695</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>774</v>
+        <v>315</v>
       </c>
       <c r="B62" t="s">
-        <v>773</v>
+        <v>873</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>775</v>
+        <v>896</v>
       </c>
       <c r="B63" t="s">
-        <v>773</v>
+        <v>596</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>497</v>
+        <v>897</v>
       </c>
       <c r="B64" t="s">
-        <v>495</v>
+        <v>596</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>498</v>
+        <v>755</v>
       </c>
       <c r="B65" t="s">
-        <v>495</v>
+        <v>694</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B66" t="s">
-        <v>495</v>
+        <v>30</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
@@ -11171,247 +11170,247 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>779</v>
+        <v>707</v>
       </c>
       <c r="B68" t="s">
-        <v>495</v>
+        <v>724</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>499</v>
+        <v>707</v>
       </c>
       <c r="B69" t="s">
-        <v>495</v>
+        <v>704</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>505</v>
-      </c>
-      <c r="B70" t="s">
-        <v>495</v>
+        <v>773</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>501</v>
+        <v>759</v>
       </c>
       <c r="B71" t="s">
-        <v>495</v>
+        <v>757</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>757</v>
+        <v>708</v>
       </c>
       <c r="B72" t="s">
-        <v>495</v>
+        <v>704</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>756</v>
+        <v>903</v>
       </c>
       <c r="B73" t="s">
-        <v>495</v>
+        <v>612</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>502</v>
+        <v>907</v>
       </c>
       <c r="B74" t="s">
-        <v>495</v>
+        <v>612</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>779</v>
+        <v>706</v>
       </c>
       <c r="B75" t="s">
-        <v>372</v>
+        <v>707</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>783</v>
-      </c>
-      <c r="B76" t="s">
+        <v>782</v>
+      </c>
+      <c r="B76" s="9" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>743</v>
+        <v>712</v>
       </c>
       <c r="B77" t="s">
-        <v>694</v>
+        <v>724</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>696</v>
+        <v>712</v>
       </c>
       <c r="B78" t="s">
-        <v>694</v>
+        <v>704</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>699</v>
+        <v>870</v>
       </c>
       <c r="B79" t="s">
-        <v>694</v>
+        <v>863</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>493</v>
-      </c>
-      <c r="B80" t="s">
-        <v>694</v>
+        <v>790</v>
+      </c>
+      <c r="B80" s="9" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>697</v>
+        <v>826</v>
       </c>
       <c r="B81" t="s">
-        <v>694</v>
+        <v>493</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>698</v>
+        <v>512</v>
       </c>
       <c r="B82" t="s">
-        <v>694</v>
+        <v>493</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>700</v>
+        <v>718</v>
       </c>
       <c r="B83" t="s">
-        <v>694</v>
+        <v>717</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>755</v>
+        <v>297</v>
       </c>
       <c r="B84" t="s">
-        <v>694</v>
+        <v>287</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>782</v>
-      </c>
-      <c r="B85" s="9" t="s">
-        <v>694</v>
+        <v>820</v>
+      </c>
+      <c r="B85" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B86" t="s">
-        <v>694</v>
+        <v>495</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
-        <v>724</v>
+        <v>779</v>
       </c>
       <c r="B87" t="s">
-        <v>694</v>
+        <v>372</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>701</v>
+        <v>495</v>
       </c>
       <c r="B88" t="s">
-        <v>694</v>
+        <v>493</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>702</v>
+        <v>499</v>
       </c>
       <c r="B89" s="7" t="s">
-        <v>694</v>
+        <v>495</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>703</v>
+        <v>499</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>694</v>
+        <v>22</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>704</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>694</v>
+        <v>883</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>350</v>
+        <v>883</v>
       </c>
       <c r="B92" t="s">
-        <v>694</v>
+        <v>612</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>781</v>
+        <v>885</v>
       </c>
       <c r="B93" t="s">
-        <v>780</v>
+        <v>596</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>726</v>
+        <v>890</v>
       </c>
       <c r="B94" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>705</v>
+        <v>892</v>
       </c>
       <c r="B95" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>725</v>
+        <v>888</v>
       </c>
       <c r="B96" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>727</v>
+        <v>894</v>
       </c>
       <c r="B97" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>697</v>
+        <v>728</v>
       </c>
       <c r="B98" t="s">
         <v>724</v>
@@ -11419,239 +11418,239 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>707</v>
+        <v>343</v>
       </c>
       <c r="B99" t="s">
-        <v>724</v>
+        <v>339</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>712</v>
+        <v>800</v>
       </c>
       <c r="B100" t="s">
-        <v>724</v>
+        <v>612</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>728</v>
+        <v>342</v>
       </c>
       <c r="B101" t="s">
-        <v>724</v>
+        <v>339</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>729</v>
+        <v>340</v>
       </c>
       <c r="B102" t="s">
-        <v>724</v>
+        <v>339</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>730</v>
+        <v>798</v>
       </c>
       <c r="B103" t="s">
-        <v>724</v>
+        <v>339</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>731</v>
+        <v>797</v>
       </c>
       <c r="B104" t="s">
-        <v>724</v>
+        <v>339</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A105" s="9" t="s">
-        <v>723</v>
+      <c r="A105" t="s">
+        <v>891</v>
       </c>
       <c r="B105" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>732</v>
+        <v>887</v>
       </c>
       <c r="B106" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>713</v>
+        <v>505</v>
       </c>
       <c r="B107" t="s">
-        <v>724</v>
+        <v>495</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>734</v>
+        <v>837</v>
       </c>
       <c r="B108" t="s">
-        <v>724</v>
+        <v>832</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>735</v>
+        <v>751</v>
       </c>
       <c r="B109" t="s">
-        <v>724</v>
+        <v>595</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>739</v>
+        <v>889</v>
       </c>
       <c r="B110" t="s">
-        <v>724</v>
+        <v>885</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>737</v>
-      </c>
-      <c r="B111" t="s">
-        <v>724</v>
+        <v>772</v>
+      </c>
+      <c r="B111" s="3" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>738</v>
-      </c>
-      <c r="B112" s="3" t="s">
-        <v>723</v>
+        <v>501</v>
+      </c>
+      <c r="B112" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>776</v>
-      </c>
-      <c r="B113" t="s">
-        <v>723</v>
+        <v>877</v>
+      </c>
+      <c r="B113" s="3" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>777</v>
-      </c>
-      <c r="B114" s="9" t="s">
-        <v>723</v>
+        <v>317</v>
+      </c>
+      <c r="B114" t="s">
+        <v>873</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>778</v>
-      </c>
-      <c r="B115" s="9" t="s">
-        <v>723</v>
+        <v>788</v>
+      </c>
+      <c r="B115" t="s">
+        <v>789</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>733</v>
+        <v>830</v>
       </c>
       <c r="B116" t="s">
-        <v>723</v>
+        <v>832</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>736</v>
-      </c>
-      <c r="B117" s="3" t="s">
-        <v>723</v>
+        <v>780</v>
+      </c>
+      <c r="B117" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>343</v>
+        <v>781</v>
       </c>
       <c r="B118" t="s">
-        <v>339</v>
+        <v>780</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>342</v>
+      <c r="A119" s="9" t="s">
+        <v>724</v>
       </c>
       <c r="B119" t="s">
-        <v>339</v>
+        <v>694</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>340</v>
+        <v>296</v>
       </c>
       <c r="B120" t="s">
-        <v>339</v>
+        <v>287</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>798</v>
+        <v>881</v>
       </c>
       <c r="B121" t="s">
-        <v>339</v>
+        <v>875</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="B122" t="s">
-        <v>339</v>
+        <v>749</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>799</v>
+        <v>902</v>
       </c>
       <c r="B123" t="s">
-        <v>339</v>
+        <v>596</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>769</v>
+        <v>821</v>
       </c>
       <c r="B124" t="s">
-        <v>770</v>
+        <v>493</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>753</v>
+        <v>918</v>
       </c>
       <c r="B125" t="s">
-        <v>702</v>
+        <v>612</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>784</v>
+        <v>701</v>
       </c>
       <c r="B126" t="s">
-        <v>703</v>
+        <v>694</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>800</v>
+        <v>825</v>
       </c>
       <c r="B127" t="s">
-        <v>612</v>
+        <v>493</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>807</v>
+        <v>825</v>
       </c>
       <c r="B128" t="s">
         <v>612</v>
@@ -11659,223 +11658,223 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>774</v>
+        <v>290</v>
       </c>
       <c r="B129" t="s">
-        <v>771</v>
+        <v>287</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>775</v>
+        <v>752</v>
       </c>
       <c r="B130" t="s">
-        <v>771</v>
+        <v>595</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>759</v>
-      </c>
-      <c r="B131" t="s">
-        <v>757</v>
+        <v>919</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>760</v>
+        <v>926</v>
       </c>
       <c r="B132" t="s">
-        <v>757</v>
+        <v>919</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>758</v>
+        <v>925</v>
       </c>
       <c r="B133" t="s">
-        <v>757</v>
+        <v>919</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>809</v>
+        <v>719</v>
       </c>
       <c r="B134" t="s">
-        <v>757</v>
+        <v>717</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>767</v>
+        <v>924</v>
       </c>
       <c r="B135" t="s">
-        <v>768</v>
+        <v>919</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>766</v>
+        <v>914</v>
       </c>
       <c r="B136" t="s">
-        <v>768</v>
+        <v>911</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>773</v>
+        <v>876</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>768</v>
+        <v>875</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>772</v>
-      </c>
-      <c r="B138" s="3" t="s">
-        <v>768</v>
+        <v>511</v>
+      </c>
+      <c r="B138" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>771</v>
-      </c>
-      <c r="B139" s="3" t="s">
-        <v>768</v>
+        <v>510</v>
+      </c>
+      <c r="B139" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>795</v>
+        <v>866</v>
       </c>
       <c r="B140" t="s">
-        <v>695</v>
+        <v>863</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>796</v>
+        <v>819</v>
       </c>
       <c r="B141" t="s">
-        <v>695</v>
+        <v>493</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>794</v>
+        <v>827</v>
       </c>
       <c r="B142" t="s">
-        <v>695</v>
+        <v>493</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>499</v>
+        <v>827</v>
       </c>
       <c r="B143" t="s">
-        <v>22</v>
+        <v>612</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>721</v>
+        <v>729</v>
       </c>
       <c r="B144" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>718</v>
+        <v>730</v>
       </c>
       <c r="B145" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>719</v>
+        <v>792</v>
       </c>
       <c r="B146" t="s">
-        <v>717</v>
+        <v>791</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>720</v>
+        <v>893</v>
       </c>
       <c r="B147" t="s">
-        <v>717</v>
+        <v>885</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>768</v>
+        <v>906</v>
       </c>
       <c r="B148" t="s">
-        <v>11</v>
+        <v>895</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>739</v>
+        <v>899</v>
       </c>
       <c r="B149" t="s">
-        <v>741</v>
+        <v>906</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>705</v>
+        <v>899</v>
       </c>
       <c r="B150" t="s">
-        <v>704</v>
+        <v>612</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>709</v>
+        <v>900</v>
       </c>
       <c r="B151" t="s">
-        <v>704</v>
+        <v>906</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>710</v>
+        <v>909</v>
       </c>
       <c r="B152" t="s">
-        <v>704</v>
+        <v>612</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>711</v>
+        <v>731</v>
       </c>
       <c r="B153" t="s">
-        <v>704</v>
+        <v>724</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>707</v>
+        <v>720</v>
       </c>
       <c r="B154" t="s">
-        <v>704</v>
+        <v>717</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>708</v>
+      <c r="A155" s="9" t="s">
+        <v>723</v>
       </c>
       <c r="B155" t="s">
-        <v>704</v>
+        <v>724</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>712</v>
+        <v>723</v>
       </c>
       <c r="B156" t="s">
         <v>704</v>
@@ -11883,567 +11882,567 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
+        <v>776</v>
+      </c>
+      <c r="B157" t="s">
         <v>723</v>
-      </c>
-      <c r="B157" t="s">
-        <v>704</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>713</v>
-      </c>
-      <c r="B158" t="s">
-        <v>704</v>
+        <v>777</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>714</v>
-      </c>
-      <c r="B159" t="s">
-        <v>704</v>
+        <v>778</v>
+      </c>
+      <c r="B159" s="9" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>715</v>
-      </c>
-      <c r="B160" t="s">
-        <v>704</v>
+        <v>793</v>
+      </c>
+      <c r="B160" s="9" t="s">
+        <v>783</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>716</v>
+        <v>829</v>
       </c>
       <c r="B161" t="s">
-        <v>704</v>
+        <v>832</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>717</v>
+        <v>764</v>
       </c>
       <c r="B162" t="s">
-        <v>704</v>
+        <v>493</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>722</v>
+        <v>293</v>
       </c>
       <c r="B163" t="s">
-        <v>704</v>
+        <v>287</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>812</v>
+        <v>886</v>
       </c>
       <c r="B164" t="s">
-        <v>811</v>
+        <v>885</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>813</v>
-      </c>
-      <c r="B165" t="s">
-        <v>811</v>
+        <v>920</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>918</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>814</v>
-      </c>
-      <c r="B166" t="s">
-        <v>612</v>
+        <v>702</v>
+      </c>
+      <c r="B166" s="9" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>814</v>
+        <v>753</v>
       </c>
       <c r="B167" t="s">
-        <v>811</v>
+        <v>702</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="B168" t="s">
-        <v>749</v>
+        <v>811</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>819</v>
+        <v>774</v>
       </c>
       <c r="B169" t="s">
-        <v>493</v>
+        <v>773</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>825</v>
+        <v>774</v>
       </c>
       <c r="B170" t="s">
-        <v>493</v>
+        <v>771</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>826</v>
+        <v>750</v>
       </c>
       <c r="B171" t="s">
-        <v>493</v>
+        <v>749</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>827</v>
+        <v>801</v>
       </c>
       <c r="B172" t="s">
-        <v>493</v>
+        <v>749</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>820</v>
+        <v>913</v>
       </c>
       <c r="B173" t="s">
-        <v>493</v>
+        <v>911</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>821</v>
+        <v>908</v>
       </c>
       <c r="B174" t="s">
-        <v>493</v>
+        <v>612</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>822</v>
+        <v>915</v>
       </c>
       <c r="B175" t="s">
-        <v>493</v>
+        <v>911</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>823</v>
+        <v>915</v>
       </c>
       <c r="B176" t="s">
-        <v>493</v>
+        <v>612</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>824</v>
+        <v>911</v>
       </c>
       <c r="B177" t="s">
-        <v>823</v>
+        <v>596</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>825</v>
-      </c>
-      <c r="B178" t="s">
-        <v>612</v>
+        <v>879</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>827</v>
+        <v>294</v>
       </c>
       <c r="B179" t="s">
-        <v>612</v>
+        <v>287</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>829</v>
+        <v>784</v>
       </c>
       <c r="B180" t="s">
-        <v>832</v>
+        <v>783</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>830</v>
+        <v>784</v>
       </c>
       <c r="B181" t="s">
-        <v>832</v>
+        <v>703</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>831</v>
+        <v>895</v>
       </c>
       <c r="B182" t="s">
-        <v>832</v>
+        <v>596</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>833</v>
+        <v>875</v>
       </c>
       <c r="B183" t="s">
-        <v>832</v>
+        <v>596</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>834</v>
-      </c>
-      <c r="B184" t="s">
-        <v>832</v>
+        <v>703</v>
+      </c>
+      <c r="B184" s="9" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>835</v>
+        <v>871</v>
       </c>
       <c r="B185" t="s">
-        <v>834</v>
+        <v>863</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>836</v>
+        <v>901</v>
       </c>
       <c r="B186" t="s">
-        <v>834</v>
+        <v>906</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>837</v>
+        <v>905</v>
       </c>
       <c r="B187" t="s">
-        <v>832</v>
+        <v>612</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>494</v>
+        <v>910</v>
       </c>
       <c r="B188" t="s">
-        <v>493</v>
+        <v>612</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
       <c r="B189" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A190" s="2" t="s">
-        <v>860</v>
+      <c r="A190" t="s">
+        <v>921</v>
       </c>
       <c r="B190" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="2" t="s">
-        <v>854</v>
+      <c r="A191" t="s">
+        <v>921</v>
       </c>
       <c r="B191" t="s">
-        <v>862</v>
+        <v>612</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A192" s="2" t="s">
-        <v>855</v>
+      <c r="A192" t="s">
+        <v>517</v>
       </c>
       <c r="B192" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A193" s="2" t="s">
-        <v>861</v>
+      <c r="A193" t="s">
+        <v>522</v>
       </c>
       <c r="B193" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A194" s="2" t="s">
-        <v>856</v>
-      </c>
-      <c r="B194" t="s">
-        <v>862</v>
+      <c r="A194" t="s">
+        <v>515</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>929</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A195" s="2" t="s">
-        <v>857</v>
+      <c r="A195" t="s">
+        <v>519</v>
       </c>
       <c r="B195" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A196" s="2" t="s">
-        <v>858</v>
+      <c r="A196" t="s">
+        <v>521</v>
       </c>
       <c r="B196" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A197" s="2" t="s">
-        <v>859</v>
+      <c r="A197" t="s">
+        <v>520</v>
       </c>
       <c r="B197" t="s">
-        <v>862</v>
+        <v>929</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A198" s="2" t="s">
-        <v>855</v>
+      <c r="A198" t="s">
+        <v>922</v>
       </c>
       <c r="B198" t="s">
-        <v>703</v>
+        <v>929</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A199" s="2" t="s">
-        <v>857</v>
+      <c r="A199" t="s">
+        <v>732</v>
       </c>
       <c r="B199" t="s">
-        <v>612</v>
+        <v>724</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>863</v>
+        <v>291</v>
       </c>
       <c r="B200" t="s">
-        <v>596</v>
+        <v>287</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>870</v>
+        <v>713</v>
       </c>
       <c r="B201" t="s">
-        <v>863</v>
+        <v>724</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>871</v>
+        <v>713</v>
       </c>
       <c r="B202" t="s">
-        <v>863</v>
+        <v>704</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>864</v>
+        <v>796</v>
       </c>
       <c r="B203" t="s">
-        <v>863</v>
+        <v>695</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>865</v>
+        <v>802</v>
       </c>
       <c r="B204" t="s">
-        <v>863</v>
+        <v>749</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>866</v>
+        <v>760</v>
       </c>
       <c r="B205" t="s">
-        <v>863</v>
+        <v>757</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>867</v>
+        <v>834</v>
       </c>
       <c r="B206" t="s">
-        <v>863</v>
+        <v>832</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>872</v>
+        <v>714</v>
       </c>
       <c r="B207" t="s">
-        <v>863</v>
+        <v>704</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>868</v>
+        <v>775</v>
       </c>
       <c r="B208" t="s">
-        <v>863</v>
+        <v>773</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>869</v>
+        <v>775</v>
       </c>
       <c r="B209" t="s">
-        <v>863</v>
+        <v>771</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>873</v>
+        <v>912</v>
       </c>
       <c r="B210" t="s">
-        <v>596</v>
+        <v>911</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>211</v>
-      </c>
-      <c r="B211" t="s">
-        <v>873</v>
+        <v>771</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>768</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>318</v>
+        <v>823</v>
       </c>
       <c r="B212" t="s">
-        <v>873</v>
+        <v>493</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>316</v>
+        <v>809</v>
       </c>
       <c r="B213" t="s">
-        <v>873</v>
+        <v>757</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>315</v>
+        <v>757</v>
       </c>
       <c r="B214" t="s">
-        <v>873</v>
+        <v>495</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>317</v>
-      </c>
-      <c r="B215" t="s">
-        <v>873</v>
+        <v>509</v>
+      </c>
+      <c r="B215" s="9" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A216" t="s">
-        <v>319</v>
+      <c r="A216" s="3" t="s">
+        <v>768</v>
       </c>
       <c r="B216" t="s">
-        <v>873</v>
+        <v>769</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>320</v>
-      </c>
-      <c r="B217" t="s">
-        <v>873</v>
+        <v>768</v>
+      </c>
+      <c r="B217" s="9" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>874</v>
+        <v>768</v>
       </c>
       <c r="B218" t="s">
-        <v>612</v>
+        <v>11</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>875</v>
+        <v>733</v>
       </c>
       <c r="B219" t="s">
-        <v>596</v>
+        <v>723</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>880</v>
-      </c>
-      <c r="B220" s="8" t="s">
-        <v>875</v>
+        <v>869</v>
+      </c>
+      <c r="B220" s="7" t="s">
+        <v>863</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>881</v>
+        <v>803</v>
       </c>
       <c r="B221" t="s">
-        <v>875</v>
+        <v>749</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>882</v>
-      </c>
-      <c r="B222" s="8" t="s">
-        <v>875</v>
+        <v>715</v>
+      </c>
+      <c r="B222" s="7" t="s">
+        <v>704</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>883</v>
-      </c>
-      <c r="B223" s="8" t="s">
-        <v>875</v>
+        <v>836</v>
+      </c>
+      <c r="B223" s="7" t="s">
+        <v>834</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>876</v>
-      </c>
-      <c r="B224" s="8" t="s">
-        <v>875</v>
+        <v>758</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>757</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>877</v>
-      </c>
-      <c r="B225" s="8" t="s">
-        <v>875</v>
+        <v>786</v>
+      </c>
+      <c r="B225" s="7" t="s">
+        <v>791</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>878</v>
-      </c>
-      <c r="B226" s="8" t="s">
-        <v>875</v>
+        <v>734</v>
+      </c>
+      <c r="B226" s="7" t="s">
+        <v>724</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="B227" s="8" t="s">
         <v>875</v>
@@ -12451,7 +12450,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="B228" s="8" t="s">
         <v>875</v>
@@ -12459,7 +12458,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="B229" t="s">
         <v>612</v>
@@ -12467,119 +12466,119 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>883</v>
+        <v>754</v>
       </c>
       <c r="B230" t="s">
-        <v>612</v>
+        <v>743</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>880</v>
+        <v>735</v>
       </c>
       <c r="B231" t="s">
-        <v>612</v>
+        <v>740</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>885</v>
+        <v>735</v>
       </c>
       <c r="B232" t="s">
-        <v>596</v>
+        <v>724</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>886</v>
+        <v>746</v>
       </c>
       <c r="B233" t="s">
-        <v>885</v>
+        <v>743</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>893</v>
+        <v>747</v>
       </c>
       <c r="B234" t="s">
-        <v>885</v>
+        <v>743</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>887</v>
+        <v>745</v>
       </c>
       <c r="B235" t="s">
-        <v>885</v>
+        <v>743</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>888</v>
+        <v>518</v>
       </c>
       <c r="B236" t="s">
-        <v>885</v>
+        <v>929</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>889</v>
+        <v>923</v>
       </c>
       <c r="B237" t="s">
-        <v>885</v>
+        <v>929</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>894</v>
+        <v>923</v>
       </c>
       <c r="B238" t="s">
-        <v>885</v>
+        <v>612</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>890</v>
+        <v>748</v>
       </c>
       <c r="B239" t="s">
-        <v>885</v>
+        <v>743</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>891</v>
+        <v>822</v>
       </c>
       <c r="B240" t="s">
-        <v>885</v>
+        <v>493</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>892</v>
+        <v>824</v>
       </c>
       <c r="B241" t="s">
-        <v>885</v>
+        <v>823</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>895</v>
+        <v>716</v>
       </c>
       <c r="B242" t="s">
-        <v>596</v>
+        <v>704</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>896</v>
+        <v>794</v>
       </c>
       <c r="B243" t="s">
-        <v>596</v>
+        <v>695</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>897</v>
+        <v>863</v>
       </c>
       <c r="B244" t="s">
         <v>596</v>
@@ -12587,207 +12586,207 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>906</v>
+        <v>864</v>
       </c>
       <c r="B245" t="s">
-        <v>895</v>
+        <v>863</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>898</v>
+        <v>865</v>
       </c>
       <c r="B246" t="s">
-        <v>906</v>
+        <v>863</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>899</v>
+        <v>868</v>
       </c>
       <c r="B247" t="s">
-        <v>906</v>
+        <v>863</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>900</v>
+        <v>917</v>
       </c>
       <c r="B248" t="s">
-        <v>906</v>
+        <v>911</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>901</v>
+        <v>316</v>
       </c>
       <c r="B249" t="s">
-        <v>906</v>
+        <v>873</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>902</v>
+        <v>717</v>
       </c>
       <c r="B250" t="s">
-        <v>596</v>
+        <v>704</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>908</v>
-      </c>
-      <c r="B251" t="s">
-        <v>612</v>
+        <v>736</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>723</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>903</v>
+        <v>739</v>
       </c>
       <c r="B252" t="s">
-        <v>612</v>
+        <v>724</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>907</v>
+        <v>739</v>
       </c>
       <c r="B253" t="s">
-        <v>612</v>
+        <v>741</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>909</v>
+        <v>765</v>
       </c>
       <c r="B254" t="s">
-        <v>612</v>
+        <v>493</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>904</v>
+        <v>762</v>
       </c>
       <c r="B255" t="s">
-        <v>612</v>
+        <v>811</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>910</v>
+        <v>318</v>
       </c>
       <c r="B256" t="s">
-        <v>612</v>
+        <v>873</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>905</v>
+        <v>319</v>
       </c>
       <c r="B257" t="s">
-        <v>612</v>
+        <v>873</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>899</v>
+        <v>873</v>
       </c>
       <c r="B258" t="s">
-        <v>612</v>
+        <v>596</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>911</v>
+        <v>812</v>
       </c>
       <c r="B259" t="s">
-        <v>596</v>
+        <v>811</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>912</v>
+        <v>756</v>
       </c>
       <c r="B260" t="s">
-        <v>911</v>
+        <v>495</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>913</v>
+        <v>320</v>
       </c>
       <c r="B261" t="s">
-        <v>911</v>
+        <v>873</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>914</v>
+        <v>722</v>
       </c>
       <c r="B262" t="s">
-        <v>911</v>
+        <v>704</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>915</v>
+        <v>292</v>
       </c>
       <c r="B263" t="s">
-        <v>911</v>
+        <v>287</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>916</v>
+        <v>787</v>
       </c>
       <c r="B264" t="s">
-        <v>911</v>
+        <v>791</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>917</v>
+        <v>211</v>
       </c>
       <c r="B265" t="s">
-        <v>911</v>
+        <v>873</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>915</v>
+        <v>927</v>
       </c>
       <c r="B266" t="s">
-        <v>612</v>
+        <v>919</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>918</v>
-      </c>
-      <c r="B267" t="s">
-        <v>612</v>
+        <v>884</v>
+      </c>
+      <c r="B267" s="3" t="s">
+        <v>875</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>919</v>
-      </c>
-      <c r="B268" s="8" t="s">
-        <v>918</v>
+        <v>884</v>
+      </c>
+      <c r="B268" s="7" t="s">
+        <v>612</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>920</v>
-      </c>
-      <c r="B269" s="8" t="s">
-        <v>918</v>
+        <v>513</v>
+      </c>
+      <c r="B269" s="7" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>929</v>
+        <v>704</v>
       </c>
       <c r="B270" t="s">
         <v>595</v>
@@ -12795,138 +12794,138 @@
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>923</v>
-      </c>
-      <c r="B271" t="s">
-        <v>929</v>
+        <v>704</v>
+      </c>
+      <c r="B271" s="9" t="s">
+        <v>694</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>517</v>
+        <v>799</v>
       </c>
       <c r="B272" t="s">
-        <v>929</v>
+        <v>339</v>
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>518</v>
+        <v>350</v>
       </c>
       <c r="B273" t="s">
-        <v>929</v>
+        <v>694</v>
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>519</v>
+        <v>737</v>
       </c>
       <c r="B274" t="s">
-        <v>929</v>
+        <v>724</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A275" t="s">
-        <v>520</v>
+      <c r="A275" s="2" t="s">
+        <v>857</v>
       </c>
       <c r="B275" t="s">
-        <v>929</v>
+        <v>862</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A276" t="s">
-        <v>521</v>
+      <c r="A276" s="2" t="s">
+        <v>857</v>
       </c>
       <c r="B276" t="s">
-        <v>929</v>
+        <v>612</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A277" t="s">
-        <v>522</v>
+      <c r="A277" s="2" t="s">
+        <v>861</v>
       </c>
       <c r="B277" t="s">
-        <v>929</v>
+        <v>862</v>
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A278" t="s">
-        <v>921</v>
+      <c r="A278" s="2" t="s">
+        <v>856</v>
       </c>
       <c r="B278" t="s">
-        <v>929</v>
+        <v>862</v>
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A279" t="s">
-        <v>922</v>
+      <c r="A279" s="2" t="s">
+        <v>854</v>
       </c>
       <c r="B279" t="s">
-        <v>929</v>
+        <v>862</v>
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A280" t="s">
-        <v>923</v>
+      <c r="A280" s="2" t="s">
+        <v>858</v>
       </c>
       <c r="B280" t="s">
-        <v>612</v>
+        <v>862</v>
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>921</v>
+        <v>862</v>
       </c>
       <c r="B281" t="s">
-        <v>612</v>
+        <v>596</v>
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A282" t="s">
-        <v>924</v>
+      <c r="A282" s="2" t="s">
+        <v>860</v>
       </c>
       <c r="B282" t="s">
-        <v>919</v>
+        <v>862</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>925</v>
+        <v>904</v>
       </c>
       <c r="B283" t="s">
-        <v>919</v>
+        <v>612</v>
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A284" t="s">
-        <v>926</v>
+      <c r="A284" s="2" t="s">
+        <v>855</v>
       </c>
       <c r="B284" t="s">
-        <v>919</v>
+        <v>862</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A285" t="s">
-        <v>927</v>
+      <c r="A285" s="2" t="s">
+        <v>855</v>
       </c>
       <c r="B285" t="s">
-        <v>919</v>
+        <v>703</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A286" t="s">
-        <v>928</v>
+      <c r="A286" s="2" t="s">
+        <v>859</v>
       </c>
       <c r="B286" t="s">
-        <v>919</v>
+        <v>862</v>
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>515</v>
-      </c>
-      <c r="B287" s="10" t="s">
-        <v>929</v>
+        <v>502</v>
+      </c>
+      <c r="B287" s="4" t="s">
+        <v>495</v>
       </c>
     </row>
   </sheetData>

</xml_diff>